<commit_message>
code refactoring and loan accounting and charges added
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/389-RBI-EI-DB-DL-REC-NON-RNI-CTPD-SAR-MD-TR-1-EarlyRePayment-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/389-RBI-EI-DB-DL-REC-NON-RNI-CTPD-SAR-MD-TR-1-EarlyRePayment-Makerepayment1.xlsx
@@ -11,34 +11,96 @@
     <sheet name="Summary" sheetId="13" r:id="rId2"/>
     <sheet name="Repayment Schedule" sheetId="17" r:id="rId3"/>
     <sheet name="Transactions" sheetId="18" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="19" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>click</t>
   </si>
   <si>
-    <t>heading</t>
-  </si>
-  <si>
     <t>makerepayment</t>
   </si>
   <si>
     <t>transactiondate</t>
   </si>
   <si>
-    <t>transactionamount</t>
-  </si>
-  <si>
     <t>Repayment</t>
   </si>
   <si>
     <t>Disbursement</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Waived</t>
+  </si>
+  <si>
+    <t>Written Off</t>
+  </si>
+  <si>
+    <t>Outstanding</t>
+  </si>
+  <si>
+    <t>Over Due</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Penalties</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Paid Date</t>
+  </si>
+  <si>
+    <t>Principal Due</t>
+  </si>
+  <si>
+    <t>Balance of Loan</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>In Advance</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Loan Balance</t>
   </si>
 </sst>
 </file>
@@ -51,12 +113,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <i/>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -99,32 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -133,6 +174,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,7 +491,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -452,12 +505,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>42019</v>
@@ -473,112 +526,113 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="A2" s="4">
         <v>10000</v>
       </c>
-      <c r="B2" s="12">
-        <v>1049.76</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12">
-        <v>8950.24</v>
-      </c>
-      <c r="F2" s="12">
-        <v>1544.81</v>
+      <c r="B2" s="6">
+        <v>841.69</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>9158.31</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1635.24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
-        <v>6718.35</v>
-      </c>
-      <c r="B3" s="13">
-        <v>552.33000000000004</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>6166.02</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1659.37</v>
+      <c r="A3" s="6">
+        <v>584.36</v>
+      </c>
+      <c r="B3" s="6">
+        <v>46.03</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>538.33000000000004</v>
+      </c>
+      <c r="F3" s="6">
+        <v>140.19999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0</v>
-      </c>
-      <c r="C4" s="13">
-        <v>0</v>
-      </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13">
-        <v>0</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
         <v>0</v>
       </c>
     </row>
@@ -589,76 +643,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
-      <c r="B2" s="7">
+      <c r="C2" s="8">
         <v>42005</v>
       </c>
-      <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="5">
+      <c r="G2" s="4">
         <v>10000</v>
       </c>
-      <c r="G2" s="6"/>
       <c r="H2" s="6">
         <v>0</v>
       </c>
@@ -680,21 +735,21 @@
       <c r="B3" s="6">
         <v>14</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>42019</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="8">
         <v>42019</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="10">
-        <v>1049.76</v>
-      </c>
-      <c r="G3" s="10">
-        <v>8950.24</v>
+      <c r="E3" s="9"/>
+      <c r="F3" s="6">
+        <v>841.69</v>
+      </c>
+      <c r="G3" s="5">
+        <v>9158.31</v>
       </c>
       <c r="H3" s="6">
-        <v>552.33000000000004</v>
+        <v>46.03</v>
       </c>
       <c r="I3" s="6">
         <v>0</v>
@@ -702,11 +757,11 @@
       <c r="J3" s="6">
         <v>0</v>
       </c>
-      <c r="K3" s="10">
-        <v>1602.09</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1602.09</v>
+      <c r="K3" s="6">
+        <v>887.72</v>
+      </c>
+      <c r="L3" s="6">
+        <v>887.72</v>
       </c>
       <c r="M3" s="6">
         <v>0</v>
@@ -725,19 +780,19 @@
       <c r="B4" s="6">
         <v>17</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>42036</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
-        <v>931.41</v>
-      </c>
-      <c r="G4" s="10">
-        <v>8018.83</v>
+        <v>831.83</v>
+      </c>
+      <c r="G4" s="5">
+        <v>8326.48</v>
       </c>
       <c r="H4" s="6">
-        <v>670.68</v>
+        <v>55.89</v>
       </c>
       <c r="I4" s="6">
         <v>0</v>
@@ -745,8 +800,8 @@
       <c r="J4" s="6">
         <v>0</v>
       </c>
-      <c r="K4" s="10">
-        <v>1602.09</v>
+      <c r="K4" s="6">
+        <v>887.72</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -757,8 +812,8 @@
       <c r="N4" s="6">
         <v>0</v>
       </c>
-      <c r="O4" s="10">
-        <v>1602.09</v>
+      <c r="O4" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -768,19 +823,19 @@
       <c r="B5" s="6">
         <v>28</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>42064</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>613.4</v>
-      </c>
-      <c r="G5" s="10">
-        <v>7405.43</v>
+        <v>803.41</v>
+      </c>
+      <c r="G5" s="5">
+        <v>7523.07</v>
       </c>
       <c r="H5" s="6">
-        <v>988.69</v>
+        <v>84.31</v>
       </c>
       <c r="I5" s="6">
         <v>0</v>
@@ -788,8 +843,8 @@
       <c r="J5" s="6">
         <v>0</v>
       </c>
-      <c r="K5" s="10">
-        <v>1602.09</v>
+      <c r="K5" s="6">
+        <v>887.72</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -800,8 +855,8 @@
       <c r="N5" s="6">
         <v>0</v>
       </c>
-      <c r="O5" s="10">
-        <v>1602.09</v>
+      <c r="O5" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -811,19 +866,19 @@
       <c r="B6" s="6">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>42095</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
-        <v>507.46</v>
-      </c>
-      <c r="G6" s="10">
-        <v>6897.97</v>
-      </c>
-      <c r="H6" s="10">
-        <v>1094.6300000000001</v>
+        <v>794.38</v>
+      </c>
+      <c r="G6" s="5">
+        <v>6728.69</v>
+      </c>
+      <c r="H6" s="6">
+        <v>93.34</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -831,8 +886,8 @@
       <c r="J6" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="10">
-        <v>1602.09</v>
+      <c r="K6" s="6">
+        <v>887.72</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -843,8 +898,8 @@
       <c r="N6" s="6">
         <v>0</v>
       </c>
-      <c r="O6" s="10">
-        <v>1602.09</v>
+      <c r="O6" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -854,19 +909,19 @@
       <c r="B7" s="6">
         <v>30</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>42125</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
-        <v>785.67</v>
-      </c>
-      <c r="G7" s="10">
-        <v>6112.3</v>
+        <v>821.35</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5907.34</v>
       </c>
       <c r="H7" s="6">
-        <v>816.42</v>
+        <v>66.37</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -874,8 +929,8 @@
       <c r="J7" s="6">
         <v>0</v>
       </c>
-      <c r="K7" s="10">
-        <v>1602.09</v>
+      <c r="K7" s="6">
+        <v>887.72</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -886,8 +941,8 @@
       <c r="N7" s="6">
         <v>0</v>
       </c>
-      <c r="O7" s="10">
-        <v>1602.09</v>
+      <c r="O7" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -897,19 +952,19 @@
       <c r="B8" s="6">
         <v>31</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>42156</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6">
-        <v>854.55</v>
-      </c>
-      <c r="G8" s="10">
-        <v>5257.75</v>
+        <v>827.51</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5079.83</v>
       </c>
       <c r="H8" s="6">
-        <v>747.54</v>
+        <v>60.21</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
@@ -917,8 +972,8 @@
       <c r="J8" s="6">
         <v>0</v>
       </c>
-      <c r="K8" s="10">
-        <v>1602.09</v>
+      <c r="K8" s="6">
+        <v>887.72</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -929,8 +984,8 @@
       <c r="N8" s="6">
         <v>0</v>
       </c>
-      <c r="O8" s="10">
-        <v>1602.09</v>
+      <c r="O8" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -940,19 +995,19 @@
       <c r="B9" s="6">
         <v>30</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>42186</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6">
-        <v>979.8</v>
-      </c>
-      <c r="G9" s="10">
-        <v>4277.95</v>
+        <v>837.62</v>
+      </c>
+      <c r="G9" s="5">
+        <v>4242.21</v>
       </c>
       <c r="H9" s="6">
-        <v>622.29</v>
+        <v>50.1</v>
       </c>
       <c r="I9" s="6">
         <v>0</v>
@@ -960,8 +1015,8 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="K9" s="10">
-        <v>1602.09</v>
+      <c r="K9" s="6">
+        <v>887.72</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -972,8 +1027,8 @@
       <c r="N9" s="6">
         <v>0</v>
       </c>
-      <c r="O9" s="10">
-        <v>1602.09</v>
+      <c r="O9" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -983,19 +1038,19 @@
       <c r="B10" s="6">
         <v>31</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>42217</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="10">
-        <v>1078.8900000000001</v>
-      </c>
-      <c r="G10" s="10">
-        <v>3199.06</v>
+      <c r="F10" s="6">
+        <v>844.48</v>
+      </c>
+      <c r="G10" s="5">
+        <v>3397.73</v>
       </c>
       <c r="H10" s="6">
-        <v>523.20000000000005</v>
+        <v>43.24</v>
       </c>
       <c r="I10" s="6">
         <v>0</v>
@@ -1003,8 +1058,8 @@
       <c r="J10" s="6">
         <v>0</v>
       </c>
-      <c r="K10" s="10">
-        <v>1602.09</v>
+      <c r="K10" s="6">
+        <v>887.72</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -1015,8 +1070,8 @@
       <c r="N10" s="6">
         <v>0</v>
       </c>
-      <c r="O10" s="10">
-        <v>1602.09</v>
+      <c r="O10" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1026,19 +1081,19 @@
       <c r="B11" s="6">
         <v>31</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>42248</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="10">
-        <v>1210.8399999999999</v>
-      </c>
-      <c r="G11" s="10">
-        <v>1988.22</v>
+      <c r="F11" s="6">
+        <v>853.09</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2544.64</v>
       </c>
       <c r="H11" s="6">
-        <v>391.25</v>
+        <v>34.630000000000003</v>
       </c>
       <c r="I11" s="6">
         <v>0</v>
@@ -1046,8 +1101,8 @@
       <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="K11" s="10">
-        <v>1602.09</v>
+      <c r="K11" s="6">
+        <v>887.72</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -1058,8 +1113,8 @@
       <c r="N11" s="6">
         <v>0</v>
       </c>
-      <c r="O11" s="10">
-        <v>1602.09</v>
+      <c r="O11" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1069,19 +1124,19 @@
       <c r="B12" s="6">
         <v>30</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="8">
         <v>42278</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="10">
-        <v>1366.77</v>
-      </c>
-      <c r="G12" s="6">
-        <v>621.45000000000005</v>
+      <c r="F12" s="6">
+        <v>862.62</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1682.02</v>
       </c>
       <c r="H12" s="6">
-        <v>235.32</v>
+        <v>25.1</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
@@ -1089,8 +1144,8 @@
       <c r="J12" s="6">
         <v>0</v>
       </c>
-      <c r="K12" s="10">
-        <v>1602.09</v>
+      <c r="K12" s="6">
+        <v>887.72</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -1101,8 +1156,8 @@
       <c r="N12" s="6">
         <v>0</v>
       </c>
-      <c r="O12" s="10">
-        <v>1602.09</v>
+      <c r="O12" s="6">
+        <v>887.72</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1112,19 +1167,19 @@
       <c r="B13" s="6">
         <v>31</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="8">
         <v>42309</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6">
-        <v>621.45000000000005</v>
+        <v>870.58</v>
       </c>
       <c r="G13" s="6">
-        <v>0</v>
+        <v>811.44</v>
       </c>
       <c r="H13" s="6">
-        <v>76</v>
+        <v>17.14</v>
       </c>
       <c r="I13" s="6">
         <v>0</v>
@@ -1133,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="6">
-        <v>697.45</v>
+        <v>887.72</v>
       </c>
       <c r="L13" s="6">
         <v>0</v>
@@ -1145,7 +1200,50 @@
         <v>0</v>
       </c>
       <c r="O13" s="6">
-        <v>697.45</v>
+        <v>887.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8">
+        <v>42339</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6">
+        <v>811.44</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>8</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>819.44</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>819.44</v>
       </c>
     </row>
   </sheetData>
@@ -1155,59 +1253,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
         <v>42019</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1602.09</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1049.76</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>887.72</v>
+      </c>
+      <c r="D2" s="6">
+        <v>841.69</v>
       </c>
       <c r="E2" s="6">
-        <v>552.33000000000004</v>
+        <v>46.03</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -1215,18 +1318,19 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="10">
-        <v>8950.24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="H2" s="5">
+        <v>9158.31</v>
+      </c>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
         <v>42005</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
         <v>10000</v>
       </c>
       <c r="D3" s="6">
@@ -1241,7 +1345,7 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>10000</v>
       </c>
     </row>
@@ -1249,46 +1353,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3">
-        <v>42060</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1934.59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>